<commit_message>
updated test data files
</commit_message>
<xml_diff>
--- a/TestData/CNBC_EndToEnd.xlsx
+++ b/TestData/CNBC_EndToEnd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgoyal0427\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B573DEB-8CF3-4A80-998E-62C7A34EE5BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6EC597-AA48-4D2B-A8F3-6A2B9478FDBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25590" windowHeight="8565" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7335" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -562,9 +562,6 @@
     <t>Opportunity Overview: Structure and Pricing Expectations.</t>
   </si>
   <si>
-    <t>Opportunity Overview: Sanctions concerns/issues?</t>
-  </si>
-  <si>
     <t>ValSanctions</t>
   </si>
   <si>
@@ -581,6 +578,9 @@
   </si>
   <si>
     <t>Financials : Capital Raise (MM)</t>
+  </si>
+  <si>
+    <t>Overview and Financials: Sanctions concerns/issues?</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:BS33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BE1" workbookViewId="0">
-      <selection activeCell="BN2" sqref="BN2"/>
+      <selection activeCell="BR2" sqref="BR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,10 +1593,10 @@
         <v>163</v>
       </c>
       <c r="BR1" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="BS1" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:71" ht="216.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,7 +1733,7 @@
         <v>117</v>
       </c>
       <c r="AS2" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AT2" s="9" t="s">
         <v>120</v>
@@ -1757,7 +1757,7 @@
         <v>133</v>
       </c>
       <c r="BA2" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BB2" s="9" t="s">
         <v>137</v>
@@ -1796,7 +1796,7 @@
         <v>156</v>
       </c>
       <c r="BN2" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="BO2" s="9" t="s">
         <v>159</v>
@@ -1808,10 +1808,10 @@
         <v>162</v>
       </c>
       <c r="BR2" s="9" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="BS2" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:71" x14ac:dyDescent="0.25">

</xml_diff>